<commit_message>
Generate ML input with median values and merge with site points
</commit_message>
<xml_diff>
--- a/workshop_feature_selection.xlsx
+++ b/workshop_feature_selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\agile2024_rf_interpretability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671BD9FB-0381-40A4-B56E-B1309F322200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF65018-D0BA-4346-9ABC-625BE70970FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -804,7 +804,7 @@
         <v>89</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -815,7 +815,7 @@
         <v>89</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -826,7 +826,7 @@
         <v>89</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -860,7 +860,7 @@
         <v>90</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>1.15162565702646E-2</v>
@@ -883,7 +883,7 @@
         <v>90</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1.76537329642707E-2</v>
@@ -906,7 +906,7 @@
         <v>90</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>1.03508968883411E-2</v>
@@ -926,7 +926,7 @@
         <v>90</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>4.3120462299322E-3</v>
@@ -949,7 +949,7 @@
         <v>91</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>9.6982864771144005E-3</v>
@@ -972,7 +972,7 @@
         <v>91</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -983,7 +983,7 @@
         <v>91</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -994,7 +994,7 @@
         <v>91</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1005,7 +1005,7 @@
         <v>92</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>1.4317221485484E-3</v>
@@ -1028,7 +1028,7 @@
         <v>92</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1050,7 +1050,7 @@
         <v>92</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1061,7 +1061,7 @@
         <v>93</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>1.7276605900401799E-2</v>
@@ -1084,7 +1084,7 @@
         <v>93</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>1.7225010821891699E-2</v>
@@ -1098,7 +1098,7 @@
         <v>93</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>6.6937120583064405E-2</v>
@@ -1115,7 +1115,7 @@
         <v>93</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>1.46835336343972E-2</v>
@@ -1135,7 +1135,7 @@
         <v>94</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1158,7 +1158,7 @@
         <v>94</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>9.3178929953102001E-3</v>
@@ -1175,7 +1175,7 @@
         <v>94</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>9.5350755958655206E-2</v>
@@ -1192,7 +1192,7 @@
         <v>94</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>1.6771734635242001E-2</v>
@@ -1217,7 +1217,7 @@
         <v>95</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>3.6106942191202203E-2</v>
@@ -1231,7 +1231,7 @@
         <v>95</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>1.6690601406095101E-2</v>
@@ -1300,7 +1300,7 @@
         <v>98</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>1.04265387447988E-2</v>
@@ -1317,7 +1317,7 @@
         <v>98</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1357,7 +1357,7 @@
         <v>98</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>4.76636071798354E-2</v>
@@ -1423,7 +1423,7 @@
         <v>100</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1434,7 +1434,7 @@
         <v>100</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>2.3559108246338702E-2</v>
@@ -1480,7 +1480,7 @@
         <v>102</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>8.4321077045824994E-3</v>
@@ -1500,7 +1500,7 @@
         <v>102</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>1.11310141587837E-2</v>
@@ -1514,7 +1514,7 @@
         <v>102</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>5.8887998848164001E-2</v>
@@ -1537,7 +1537,7 @@
         <v>102</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>4.2986806619157297E-2</v>
@@ -1577,7 +1577,7 @@
         <v>104</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
         <v>8.3375716337524899E-2</v>
@@ -1600,7 +1600,7 @@
         <v>104</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
         <v>0.1067460267881114</v>
@@ -1620,7 +1620,7 @@
         <v>105</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -1643,7 +1643,7 @@
         <v>105</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1689,7 +1689,7 @@
         <v>105</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>1.1550733077265399E-2</v>
@@ -1706,7 +1706,7 @@
         <v>106</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1720,7 +1720,7 @@
         <v>106</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -1742,7 +1742,7 @@
         <v>106</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>3.6893275810507498E-2</v>
@@ -1765,7 +1765,7 @@
         <v>107</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -1776,7 +1776,7 @@
         <v>107</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>2.3665483730014999E-3</v>
@@ -1813,7 +1813,7 @@
         <v>107</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
         <v>1.8080716967985799E-2</v>
@@ -1836,7 +1836,7 @@
         <v>108</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
         <v>7.5841612171769998E-4</v>
@@ -1859,7 +1859,7 @@
         <v>108</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>9.0998563774394008E-3</v>
@@ -1893,7 +1893,7 @@
         <v>108</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -1904,7 +1904,7 @@
         <v>109</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>6.9621446001811998E-3</v>
@@ -1927,7 +1927,7 @@
         <v>110</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -1938,7 +1938,7 @@
         <v>110</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>1.58490691867876E-2</v>
@@ -1981,7 +1981,7 @@
         <v>110</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -1992,7 +1992,7 @@
         <v>74</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <v>5.4169918016053899E-2</v>
@@ -2015,7 +2015,7 @@
         <v>111</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>1.0988381831077899E-2</v>
@@ -2058,7 +2058,7 @@
         <v>111</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <v>2.3678234801679701E-2</v>
@@ -2081,7 +2081,7 @@
         <v>112</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -2104,7 +2104,7 @@
         <v>112</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>4.1468497789956E-3</v>
@@ -2124,7 +2124,7 @@
         <v>112</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>3.3232375732994E-2</v>
@@ -2138,7 +2138,7 @@
         <v>112</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2149,7 +2149,7 @@
         <v>113</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>9.0803062316911001E-3</v>
@@ -2166,7 +2166,7 @@
         <v>113</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>2.5221861819150902E-2</v>
@@ -2209,7 +2209,7 @@
         <v>113</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>